<commit_message>
Modified template excel spreadsheet
</commit_message>
<xml_diff>
--- a/ionic/resources/excel/Question-Options.xlsx
+++ b/ionic/resources/excel/Question-Options.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Option1</t>
   </si>
@@ -407,7 +407,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -483,28 +483,28 @@
       <c r="A7">
         <v>24</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>27</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
         <v>2</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
+      <c r="D8" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>